<commit_message>
Modified css and layout
</commit_message>
<xml_diff>
--- a/docs/Test-Cases-Stauts.xlsx
+++ b/docs/Test-Cases-Stauts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Title</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t xml:space="preserve">Implement sorting that changes with a dropdown. The sort options should be title and created_date. </t>
+  </si>
+  <si>
+    <t>Implement a notification to tell the user that edits have been successfully saved.</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,8 +657,12 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
   </sheetData>

</xml_diff>